<commit_message>
accepting manual_iop column and working for columns that doesn't have manual iop value
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">ground_level_end</t>
   </si>
   <si>
-    <t xml:space="preserve">old_iop</t>
+    <t xml:space="preserve">manual_iop</t>
   </si>
   <si>
     <t xml:space="preserve">J-4174</t>
@@ -3961,9 +3961,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>191880</xdr:colOff>
+      <xdr:colOff>191160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3973,7 +3973,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2862360" y="5087520"/>
-          <a:ext cx="80280" cy="110520"/>
+          <a:ext cx="79560" cy="109800"/>
         </a:xfrm>
         <a:prstGeom prst="star5">
           <a:avLst>
@@ -4018,9 +4018,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>205920</xdr:colOff>
+      <xdr:colOff>205200</xdr:colOff>
       <xdr:row>1191</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4030,7 +4030,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2862360" y="215582040"/>
-          <a:ext cx="94320" cy="105120"/>
+          <a:ext cx="93600" cy="104400"/>
         </a:xfrm>
         <a:prstGeom prst="star5">
           <a:avLst>
@@ -4248,8 +4248,8 @@
   </sheetPr>
   <dimension ref="A1:G1250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F231" activeCellId="0" sqref="F231"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4920,9 +4920,7 @@
       <c r="F29" s="5" t="n">
         <v>206.98</v>
       </c>
-      <c r="G29" s="6" t="n">
-        <v>1400</v>
-      </c>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">

</xml_diff>